<commit_message>
Committing changes to switch over to laptop
</commit_message>
<xml_diff>
--- a/Relevant Documents/Dataset_statistics.xlsx
+++ b/Relevant Documents/Dataset_statistics.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -219,7 +218,7 @@
                   <c:v>32216</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1782.8</c:v>
+                  <c:v>1659.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7450.4285714285716</c:v>
@@ -760,6 +759,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="342084320"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1693,19 +1693,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="27" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="31" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
@@ -1763,14 +1763,14 @@
       </c>
       <c r="C2" s="1">
         <f>B2/$B$9</f>
-        <v>0.49119472149353505</v>
+        <v>0.49714949964621452</v>
       </c>
       <c r="E2">
         <v>110179</v>
       </c>
       <c r="F2" s="1">
         <f>E2/$E$9</f>
-        <v>0.37182437904967602</v>
+        <v>0.37195492478461661</v>
       </c>
       <c r="H2">
         <f>SUM(B2,E2)</f>
@@ -1778,10 +1778,10 @@
       </c>
       <c r="I2" s="1">
         <f>H2/$H$9</f>
-        <v>0.43191644824604331</v>
+        <v>0.4346128032431375</v>
       </c>
       <c r="P2" s="2">
-        <f>H2/S2</f>
+        <f t="shared" ref="P2:P7" si="0">H2/S2</f>
         <v>32216</v>
       </c>
       <c r="S2">
@@ -1793,30 +1793,30 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>21442</v>
+        <v>17844</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C7" si="0">B3/$B$9</f>
-        <v>7.1381013888703937E-2</v>
+        <f t="shared" ref="C3:C7" si="1">B3/$B$9</f>
+        <v>6.0123319518851713E-2</v>
       </c>
       <c r="E3">
-        <v>32042</v>
+        <v>31938</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F7" si="1">E3/$E$9</f>
-        <v>0.10813309935205184</v>
+        <f t="shared" ref="F3:F7" si="2">E3/$E$9</f>
+        <v>0.10781996921165636</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H7" si="2">SUM(B3,E3)</f>
-        <v>53484</v>
+        <f t="shared" ref="H3:H7" si="3">SUM(B3,E3)</f>
+        <v>49782</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I7" si="3">H3/$H$9</f>
-        <v>8.9631779697942712E-2</v>
+        <f t="shared" ref="I3:I7" si="4">H3/$H$9</f>
+        <v>8.3948560385561019E-2</v>
       </c>
       <c r="P3" s="2">
-        <f>H3/S3</f>
-        <v>1782.8</v>
+        <f t="shared" si="0"/>
+        <v>1659.4</v>
       </c>
       <c r="S3">
         <v>30</v>
@@ -1830,26 +1830,26 @@
         <v>25551</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>8.505998908078885E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.6091175578692003E-2</v>
       </c>
       <c r="E4">
         <v>26602</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="1"/>
-        <v>8.9774568034557231E-2</v>
+        <f t="shared" si="2"/>
+        <v>8.9806087449698868E-2</v>
       </c>
       <c r="H4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52153</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="3"/>
-        <v>8.740120796101275E-2</v>
+        <f t="shared" si="4"/>
+        <v>8.7946833590216628E-2</v>
       </c>
       <c r="P4" s="2">
-        <f>H4/S4</f>
+        <f t="shared" si="0"/>
         <v>7450.4285714285716</v>
       </c>
       <c r="S4">
@@ -1864,26 +1864,26 @@
         <v>6127</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>2.0396953273765929E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0644226557498566E-2</v>
       </c>
       <c r="E5">
         <v>5396</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8210043196544276E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.8216436654333323E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11523</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="3"/>
-        <v>1.9310952760814334E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.9431506595211517E-2</v>
       </c>
       <c r="P5" s="2">
-        <f>H5/S5</f>
+        <f t="shared" si="0"/>
         <v>5761.5</v>
       </c>
       <c r="S5">
@@ -1898,26 +1898,26 @@
         <v>50742</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.16892152815691705</v>
+        <f t="shared" si="1"/>
+        <v>0.17096937228343273</v>
       </c>
       <c r="E6">
         <v>53937</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>0.18202281317494601</v>
+        <f t="shared" si="2"/>
+        <v>0.18208672050125585</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104679</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="3"/>
-        <v>0.17542751228406525</v>
+        <f t="shared" si="4"/>
+        <v>0.17652266587521881</v>
       </c>
       <c r="P6" s="2">
-        <f>H6/S6</f>
+        <f t="shared" si="0"/>
         <v>20935.8</v>
       </c>
       <c r="S6">
@@ -1932,26 +1932,26 @@
         <v>48977</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.16304579410628919</v>
+        <f t="shared" si="1"/>
+        <v>0.16502240641531049</v>
       </c>
       <c r="E7">
         <v>68164</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.23003509719222462</v>
+        <f t="shared" si="2"/>
+        <v>0.23011586139843898</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117141</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="3"/>
-        <v>0.19631209905012167</v>
+        <f t="shared" si="4"/>
+        <v>0.19753763031065452</v>
       </c>
       <c r="P7" s="2">
-        <f>H7/S7</f>
+        <f t="shared" si="0"/>
         <v>6507.833333333333</v>
       </c>
       <c r="S7">
@@ -1961,15 +1961,15 @@
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>SUM(B2:B7)</f>
-        <v>300388</v>
+        <v>296790</v>
       </c>
       <c r="E9">
         <f>SUM(E2:E7)</f>
-        <v>296320</v>
+        <v>296216</v>
       </c>
       <c r="H9">
         <f>SUM(H2:H7)</f>
-        <v>596708</v>
+        <v>593006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>